<commit_message>
lr: update the tas forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Liberia/2024/lr_lf_tas_2410_1_sit_part.xlsx
+++ b/LF/TAS/Liberia/2024/lr_lf_tas_2410_1_sit_part.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Liberia\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9127AD-5C7B-4AC5-A02F-3D8506F71304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1582553-EA8E-4BB5-B129-D5D32B93B343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2423,7 +2423,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3097,7 +3097,7 @@
       </c>
       <c r="D30" s="5"/>
       <c r="H30" s="4" t="s">
-        <v>552</v>
+        <v>97</v>
       </c>
       <c r="J30" s="5"/>
     </row>

</xml_diff>